<commit_message>
Add pre-vote raw pres variable
</commit_message>
<xml_diff>
--- a/data-raw/ANES Codebook Metadata.xlsx
+++ b/data-raw/ANES Codebook Metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\GitHub\tidy-survey-book\DataCleaningScripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\GitHub\srvyrexploR\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C58B60-1554-44E3-8D11-0381B20A83D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548B403F-97AB-45F9-B76F-26312EF29FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87126550-46F9-45BE-84C8-25ED2D9052A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
   <si>
     <t>V200010b</t>
   </si>
@@ -448,6 +448,12 @@
   </si>
   <si>
     <t>CaseID</t>
+  </si>
+  <si>
+    <t>V201028</t>
+  </si>
+  <si>
+    <t>PRE: DID R VOTE FOR PRESIDENT</t>
   </si>
 </sst>
 </file>
@@ -813,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B975FC07-EEF0-4FEF-BAF7-7B34D90FE001}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,57 +938,60 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="E9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
       </c>
       <c r="E11" t="s">
         <v>136</v>
@@ -990,27 +999,24 @@
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E13" t="s">
         <v>136</v>
@@ -1018,30 +1024,27 @@
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>70</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E15" t="s">
         <v>136</v>
@@ -1049,50 +1052,50 @@
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="E17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E18" t="s">
         <v>136</v>
@@ -1100,114 +1103,117 @@
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>81</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>101</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>82</v>
       </c>
-      <c r="E20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="E21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E21" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="E22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="E23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E23" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="E24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="E25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E26" t="s">
         <v>136</v>
@@ -1215,72 +1221,72 @@
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>38</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E27" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="E28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>39</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>53</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>103</v>
       </c>
-      <c r="E28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="E29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>104</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E29" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>114</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" t="s">
-        <v>115</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>107</v>
@@ -1291,10 +1297,10 @@
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>107</v>
@@ -1305,10 +1311,10 @@
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>107</v>
@@ -1317,12 +1323,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>107</v>
@@ -1331,74 +1337,74 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>40</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="E36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>125</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>120</v>
       </c>
-      <c r="E36" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="E37" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>17</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>121</v>
-      </c>
-      <c r="B38" t="s">
-        <v>127</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="E38" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>18</v>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E39" t="s">
         <v>139</v>
@@ -1406,63 +1412,77 @@
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E40" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>130</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>131</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E41" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" t="s">
-        <v>43</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>129</v>
       </c>
       <c r="E42" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>44</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>